<commit_message>
changed df creation to account for partys with + in their name. looped over all countries. Currently takes 2 minutes
</commit_message>
<xml_diff>
--- a/results/Preliminaries-Austria.xlsx
+++ b/results/Preliminaries-Austria.xlsx
@@ -59,31 +59,31 @@
     <t>2019</t>
   </si>
   <si>
-    <t>FPÖ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GA </t>
-  </si>
-  <si>
-    <t>LIF</t>
-  </si>
-  <si>
-    <t>SPÖ</t>
-  </si>
-  <si>
-    <t>ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ</t>
-  </si>
-  <si>
-    <t>FRA</t>
-  </si>
-  <si>
-    <t>NEO</t>
-  </si>
-  <si>
-    <t>PIL</t>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)</t>
+  </si>
+  <si>
+    <t>LIF - Liberal Forum (Liberales Forum, LIF)</t>
+  </si>
+  <si>
+    <t>SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)</t>
   </si>
   <si>
     <t>Key</t>
@@ -113,310 +113,310 @@
     <t>Key_2</t>
   </si>
   <si>
-    <t xml:space="preserve">FPÖ+GA </t>
-  </si>
-  <si>
-    <t>FPÖ+LIF</t>
-  </si>
-  <si>
-    <t>FPÖ+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>GA +LIF</t>
-  </si>
-  <si>
-    <t>GA +SPÖ</t>
-  </si>
-  <si>
-    <t>GA +ÖVP</t>
-  </si>
-  <si>
-    <t>LIF+SPÖ</t>
-  </si>
-  <si>
-    <t>LIF+ÖVP</t>
-  </si>
-  <si>
-    <t>SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +LIF</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+LIF+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+LIF+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>GA +LIF+SPÖ</t>
-  </si>
-  <si>
-    <t>GA +LIF+ÖVP</t>
-  </si>
-  <si>
-    <t>GA +SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>LIF+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +LIF+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +LIF+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+LIF+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>GA +LIF+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +LIF+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ+FPÖ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BZÖ+GA </t>
-  </si>
-  <si>
-    <t>BZÖ+SPÖ</t>
-  </si>
-  <si>
-    <t>BZÖ+ÖVP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BZÖ+FPÖ+GA </t>
-  </si>
-  <si>
-    <t>BZÖ+FPÖ+SPÖ</t>
-  </si>
-  <si>
-    <t>BZÖ+FPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ+GA +SPÖ</t>
-  </si>
-  <si>
-    <t>BZÖ+GA +ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ+FPÖ+GA +SPÖ</t>
-  </si>
-  <si>
-    <t>BZÖ+FPÖ+GA +ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ+FPÖ+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ+GA +SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>BZÖ+FPÖ+GA +SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRA+GA </t>
-  </si>
-  <si>
-    <t>FRA+NEO</t>
-  </si>
-  <si>
-    <t>FRA+SPÖ</t>
-  </si>
-  <si>
-    <t>FRA+ÖVP</t>
-  </si>
-  <si>
-    <t>GA +NEO</t>
-  </si>
-  <si>
-    <t>NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>NEO+ÖVP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPÖ+FRA+GA </t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+NEO</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +NEO</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO+ÖVP</t>
-  </si>
-  <si>
-    <t>FRA+GA +NEO</t>
-  </si>
-  <si>
-    <t>FRA+GA +SPÖ</t>
-  </si>
-  <si>
-    <t>FRA+GA +ÖVP</t>
-  </si>
-  <si>
-    <t>FRA+NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>FRA+NEO+ÖVP</t>
-  </si>
-  <si>
-    <t>FRA+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>GA +NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>GA +NEO+ÖVP</t>
-  </si>
-  <si>
-    <t>NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+GA +NEO</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+GA +SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+GA +ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+NEO+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +NEO+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FRA+GA +NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>FRA+GA +NEO+ÖVP</t>
-  </si>
-  <si>
-    <t>FRA+GA +SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FRA+NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>GA +NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+GA +NEO+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+GA +NEO+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+GA +SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+GA +NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FRA+GA +NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+FRA+GA +NEO+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+PIL</t>
-  </si>
-  <si>
-    <t>NEO+PIL</t>
-  </si>
-  <si>
-    <t>PIL+SPÖ</t>
-  </si>
-  <si>
-    <t>PIL+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO+PIL</t>
-  </si>
-  <si>
-    <t>FPÖ+PIL+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+PIL+ÖVP</t>
-  </si>
-  <si>
-    <t>NEO+PIL+SPÖ</t>
-  </si>
-  <si>
-    <t>NEO+PIL+ÖVP</t>
-  </si>
-  <si>
-    <t>PIL+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO+PIL+SPÖ</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO+PIL+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+PIL+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>NEO+PIL+SPÖ+ÖVP</t>
-  </si>
-  <si>
-    <t>FPÖ+NEO+PIL+SPÖ+ÖVP</t>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+LIF - Liberal Forum (Liberales Forum, LIF)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>LIF - Liberal Forum (Liberales Forum, LIF)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+LIF - Liberal Forum (Liberales Forum, LIF)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+LIF - Liberal Forum (Liberales Forum, LIF)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>BZÖ - Alliance for the Future of Austria  (Bündnis Zukunft Österreich , BZÖ)+FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+FRANK - Team Frank Stronach (Team Frank Stronach, FRANK)+GA - The Greens-Green Alternative (Die Grünen-Die Grüne Alternative, GA)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)</t>
+  </si>
+  <si>
+    <t>PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
+  </si>
+  <si>
+    <t>FPÖ - Freedom Party of Austria (Freiheitliche Partei Österreichs, FPÖ)+NEOS - New Austria and Liberal Forum (NEOS Das Neue Österreich und Liberales Forum, NEOS)+PILZ - Peter Pilz List (Liste Peter Pilz, PILZ)+SPÖ - Social Democratic Party of Austria  (Sozialdemokratische Partei Österreichs, SPÖ)+ÖVP - Austrian People's Party  (Österreichische Volkspartei, ÖVP)</t>
   </si>
 </sst>
 </file>

</xml_diff>